<commit_message>
Update Excel Mapper to allow you to Map multiple column names for uisng the same class with multiple excel files or tabs
</commit_message>
<xml_diff>
--- a/src/Root16.Sprout.Excel.Sample/Data/test.xlsx
+++ b/src/Root16.Sprout.Excel.Sample/Data/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyenterbriars\dev\sprout\src\Root16.Sprout.Excel.Sample\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnPeters\source\repos\Root16\sprout\src\Root16.Sprout.Excel.Sample\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236FB443-AF76-49A3-B99B-B8D75EDFCB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874F0B8A-8BE9-43A6-B065-4A561E1592F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CEB87106-A47A-4C98-9558-1BFE9B2A2111}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{CEB87106-A47A-4C98-9558-1BFE9B2A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Account Name</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>A simple WhoLeNumber</t>
+  </si>
+  <si>
+    <t>Account Name 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>My Cool Float 1</t>
+  </si>
+  <si>
+    <t>A Decimal Here??? 1</t>
+  </si>
+  <si>
+    <t>A simple WhoLeNumber 1</t>
   </si>
 </sst>
 </file>
@@ -443,37 +458,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BB2943-661C-4C64-9509-0DD82479A2B9}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -490,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -507,7 +522,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -526,6 +541,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -533,20 +549,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB80B9F-6FD1-475B-9E6A-A17FA4DA8102}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>